<commit_message>
Garden Excel Sheet Updated...
</commit_message>
<xml_diff>
--- a/back-end/Garden/GardenData.xlsx
+++ b/back-end/Garden/GardenData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wed-project\wedding_planner\back-end\Garden\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DeadZoneMajorProject\wedding_planner\back-end\Garden\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F4D2D4-F1A4-486C-822F-8F70BA542ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3A48AC-38A8-47CA-AA9A-B88BFD096ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
   <si>
     <t>imageUrl</t>
   </si>
@@ -58,52 +58,109 @@
     <t>Ravi Digital Studio</t>
   </si>
   <si>
-    <t>address</t>
-  </si>
-  <si>
     <t>rating</t>
   </si>
   <si>
     <t>description</t>
   </si>
   <si>
-    <t xml:space="preserve">Indore </t>
-  </si>
-  <si>
-    <t>Bhopal</t>
-  </si>
-  <si>
-    <t>Madhya Pradesh</t>
-  </si>
-  <si>
-    <t>Shajapur</t>
-  </si>
-  <si>
-    <t>Up</t>
-  </si>
-  <si>
-    <t>Delhi</t>
-  </si>
-  <si>
-    <t>Kashmir</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
     <t>price</t>
   </si>
   <si>
-    <t xml:space="preserve">Lorem, ipsum dolor sit amet consectetur adipisicing elit. Doloribus omnis, autem deserunt dolorem praesentium </t>
-  </si>
-  <si>
     <t xml:space="preserve">Balaji </t>
   </si>
   <si>
-    <t>https://images.wedmegood.com/images/handpicked-badge-web.png</t>
-  </si>
-  <si>
     <t>capacity</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>Vijay Nagar,Indore</t>
+  </si>
+  <si>
+    <t>Annapurna,Indore</t>
+  </si>
+  <si>
+    <t>Bhawarkua,Indore</t>
+  </si>
+  <si>
+    <t>Rajwada,Indore</t>
+  </si>
+  <si>
+    <t>MR 10 Road,Indore</t>
+  </si>
+  <si>
+    <t>Navlakha,Indore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lokmanya Nagar, Indore </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scheme No. 54, Indore </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scheme No. 74, Indore </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sukhliya, Indore </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Airport Road, Indore </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nipania, Indore </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tilak Nagar, Indore </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palasia, Indore </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pardesipura, Indore </t>
+  </si>
+  <si>
+    <t>https://image.wedmegood.com/resized/450X/uploads/project/831/1433411649_PCS_2243.JPG</t>
+  </si>
+  <si>
+    <t>https://image.wedmegood.com/resized/450X/uploads/project/61882/1567934592_IMG_0762.jpg</t>
+  </si>
+  <si>
+    <t>https://image.wedmegood.com/resized/450X/uploads/images/77f703de58cf4ef9991bfb8d87c88455realwedding/1438593529_20_ADI_3823.jpg</t>
+  </si>
+  <si>
+    <t>https://image.wedmegood.com/resized/450X/uploads/images/29119e3236c141a9b651a11dcd7cfb71realwedding/1469086674_1467716476_Engagement_32.jpg</t>
+  </si>
+  <si>
+    <t>https://image.wedmegood.com/resized/450X/uploads/project/8506/1472060443_0F4A8844.jpg</t>
+  </si>
+  <si>
+    <t>https://image.wedmegood.com/resized/450X/uploads/project/21549/1506077884_12983409_10156785782520057_8025179449844878961_o.jpg</t>
+  </si>
+  <si>
+    <t>https://image.wedmegood.com/resized/450X/uploads/project/1454/1439182065_IMG_2906.JPG</t>
+  </si>
+  <si>
+    <t>https://image.wedmegood.com/resized/450X/uploads/project/8711/1472478658_13265926_10154832363738222_9216591246948716119_n.jpg</t>
+  </si>
+  <si>
+    <t>https://image.wedmegood.com/resized/450X/uploads/project/20246/1526591357_30762714_2017645688562010_9202978509931151360_n.jpg</t>
+  </si>
+  <si>
+    <t>https://image.wedmegood.com/resized/450X/uploads/member/12191/1429696411_upo.jpg</t>
+  </si>
+  <si>
+    <t>contactNo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balaji Garden in Indore, also known as Shree Balaji Mangal Parisar, is a well-regarded wedding venue situated in Gumasta Nagar. This venue offers a spacious lawn that can accommodate up to 1,000 guests, making it ideal for large gatherings and weddings. The lush green lawn provides a serene backdrop, perfect for outdoor ceremonies and receptions​ </t>
+  </si>
+  <si>
+    <t>Raj Hans Garden</t>
   </si>
 </sst>
 </file>
@@ -394,463 +451,505 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J307"/>
+  <dimension ref="A1:H307"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="24.6328125" customWidth="1"/>
-    <col min="3" max="3" width="80.1796875" customWidth="1"/>
-    <col min="4" max="4" width="20.81640625" customWidth="1"/>
-    <col min="6" max="6" width="51" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" customWidth="1"/>
+    <col min="6" max="6" width="83.7265625" customWidth="1"/>
+    <col min="7" max="7" width="36.26953125" customWidth="1"/>
+    <col min="11" max="11" width="25.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="7">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2">
+        <v>500</v>
+      </c>
+      <c r="D2">
+        <v>8889344700</v>
+      </c>
+      <c r="E2" s="7">
         <v>40000</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="5">
+      <c r="F2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="5">
         <v>4.3</v>
       </c>
-      <c r="F2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>700</v>
+      </c>
+      <c r="D3">
+        <v>9993706123</v>
+      </c>
+      <c r="E3" s="7">
         <v>70000</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="5">
+      <c r="F3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="5">
         <v>3.3</v>
       </c>
-      <c r="F3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4">
+        <v>1000</v>
+      </c>
+      <c r="D4">
+        <v>9990744744</v>
+      </c>
+      <c r="E4" s="7">
         <v>50000</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="5">
+      <c r="F4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="5">
         <v>5</v>
       </c>
-      <c r="F4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <v>5000</v>
+      </c>
+      <c r="D5">
+        <v>8228690033</v>
+      </c>
+      <c r="E5" s="7">
         <v>30000</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="5">
+      <c r="F5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="5">
         <v>2.9</v>
       </c>
-      <c r="F5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6">
+        <v>800</v>
+      </c>
+      <c r="D6">
+        <v>8779390055</v>
+      </c>
+      <c r="E6" s="7">
         <v>450000</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="5">
+      <c r="F6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="5">
         <v>5</v>
       </c>
-      <c r="F6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7">
+        <v>10000</v>
+      </c>
+      <c r="D7">
+        <v>8580897517</v>
+      </c>
+      <c r="E7" s="7">
         <v>362000</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="5">
+      <c r="F7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="5">
         <v>4.0999999999999996</v>
       </c>
-      <c r="F7" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8">
+        <v>2000</v>
+      </c>
+      <c r="D8">
+        <v>8382404979</v>
+      </c>
+      <c r="E8" s="7">
         <v>440000</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="5">
+      <c r="F8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="5">
         <v>3.2</v>
       </c>
-      <c r="F8" t="s">
-        <v>24</v>
-      </c>
-      <c r="J8">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9">
+        <v>2400</v>
+      </c>
+      <c r="D9">
+        <v>8183912441</v>
+      </c>
+      <c r="E9" s="7">
         <v>518000</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="5">
+      <c r="F9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="5">
         <v>4.5</v>
       </c>
-      <c r="F9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J9">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10">
+        <v>5400</v>
+      </c>
+      <c r="D10">
+        <v>7985419903</v>
+      </c>
+      <c r="E10" s="7">
         <v>596000</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="5">
+      <c r="F10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="5">
         <v>5</v>
       </c>
-      <c r="F10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J10">
-        <v>5400</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11">
+        <v>3800</v>
+      </c>
+      <c r="D11">
+        <v>7786927365</v>
+      </c>
+      <c r="E11" s="7">
         <v>674000</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="5">
+      <c r="F11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="5">
         <v>2</v>
       </c>
-      <c r="F11" t="s">
-        <v>24</v>
-      </c>
-      <c r="J11">
-        <v>3800</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12">
+        <v>3200</v>
+      </c>
+      <c r="D12">
+        <v>7588434827</v>
+      </c>
+      <c r="E12" s="7">
         <v>752000</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="5">
+      <c r="F12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="5">
         <v>5</v>
       </c>
-      <c r="F12" t="s">
-        <v>24</v>
-      </c>
-      <c r="J12">
-        <v>3200</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13">
+        <v>1300</v>
+      </c>
+      <c r="D13">
+        <v>7389942289</v>
+      </c>
+      <c r="E13" s="7">
         <v>830000</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="5">
+      <c r="F13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="5">
         <v>3</v>
       </c>
-      <c r="F13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J13">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14">
+        <v>5000</v>
+      </c>
+      <c r="D14">
+        <v>7191449751</v>
+      </c>
+      <c r="E14" s="7">
         <v>908000</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="5">
+      <c r="F14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="5">
         <v>4</v>
       </c>
-      <c r="F14" t="s">
-        <v>24</v>
-      </c>
-      <c r="J14">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15">
+        <v>6000</v>
+      </c>
+      <c r="D15">
+        <v>6992957213</v>
+      </c>
+      <c r="E15" s="7">
         <v>986000</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="5">
+      <c r="F15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15" s="5">
         <v>3</v>
       </c>
-      <c r="F15" t="s">
-        <v>24</v>
-      </c>
-      <c r="J15">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="7">
+    </row>
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16">
+        <v>7000</v>
+      </c>
+      <c r="D16">
+        <v>6794464675</v>
+      </c>
+      <c r="E16" s="7">
         <v>1064000</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="5">
+      <c r="F16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" s="5">
         <v>5</v>
-      </c>
-      <c r="F16" t="s">
-        <v>24</v>
-      </c>
-      <c r="J16">
-        <v>7000</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="8"/>
+      <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="8"/>
+      <c r="C18" s="2"/>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
-      <c r="C19" s="8"/>
+      <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="8"/>
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
-      <c r="C21" s="8"/>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
-      <c r="C22" s="8"/>
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
       <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
       <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
-      <c r="C28" s="2"/>
       <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
some changes in Garden Model
</commit_message>
<xml_diff>
--- a/back-end/Garden/GardenData.xlsx
+++ b/back-end/Garden/GardenData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wed-project\wedding_planner\back-end\Garden\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DeadZoneMajorProject\wedding_planner\back-end\Garden\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F4D2D4-F1A4-486C-822F-8F70BA542ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3A48AC-38A8-47CA-AA9A-B88BFD096ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
   <si>
     <t>imageUrl</t>
   </si>
@@ -58,52 +58,109 @@
     <t>Ravi Digital Studio</t>
   </si>
   <si>
-    <t>address</t>
-  </si>
-  <si>
     <t>rating</t>
   </si>
   <si>
     <t>description</t>
   </si>
   <si>
-    <t xml:space="preserve">Indore </t>
-  </si>
-  <si>
-    <t>Bhopal</t>
-  </si>
-  <si>
-    <t>Madhya Pradesh</t>
-  </si>
-  <si>
-    <t>Shajapur</t>
-  </si>
-  <si>
-    <t>Up</t>
-  </si>
-  <si>
-    <t>Delhi</t>
-  </si>
-  <si>
-    <t>Kashmir</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
     <t>price</t>
   </si>
   <si>
-    <t xml:space="preserve">Lorem, ipsum dolor sit amet consectetur adipisicing elit. Doloribus omnis, autem deserunt dolorem praesentium </t>
-  </si>
-  <si>
     <t xml:space="preserve">Balaji </t>
   </si>
   <si>
-    <t>https://images.wedmegood.com/images/handpicked-badge-web.png</t>
-  </si>
-  <si>
     <t>capacity</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>Vijay Nagar,Indore</t>
+  </si>
+  <si>
+    <t>Annapurna,Indore</t>
+  </si>
+  <si>
+    <t>Bhawarkua,Indore</t>
+  </si>
+  <si>
+    <t>Rajwada,Indore</t>
+  </si>
+  <si>
+    <t>MR 10 Road,Indore</t>
+  </si>
+  <si>
+    <t>Navlakha,Indore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lokmanya Nagar, Indore </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scheme No. 54, Indore </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scheme No. 74, Indore </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sukhliya, Indore </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Airport Road, Indore </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nipania, Indore </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tilak Nagar, Indore </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palasia, Indore </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pardesipura, Indore </t>
+  </si>
+  <si>
+    <t>https://image.wedmegood.com/resized/450X/uploads/project/831/1433411649_PCS_2243.JPG</t>
+  </si>
+  <si>
+    <t>https://image.wedmegood.com/resized/450X/uploads/project/61882/1567934592_IMG_0762.jpg</t>
+  </si>
+  <si>
+    <t>https://image.wedmegood.com/resized/450X/uploads/images/77f703de58cf4ef9991bfb8d87c88455realwedding/1438593529_20_ADI_3823.jpg</t>
+  </si>
+  <si>
+    <t>https://image.wedmegood.com/resized/450X/uploads/images/29119e3236c141a9b651a11dcd7cfb71realwedding/1469086674_1467716476_Engagement_32.jpg</t>
+  </si>
+  <si>
+    <t>https://image.wedmegood.com/resized/450X/uploads/project/8506/1472060443_0F4A8844.jpg</t>
+  </si>
+  <si>
+    <t>https://image.wedmegood.com/resized/450X/uploads/project/21549/1506077884_12983409_10156785782520057_8025179449844878961_o.jpg</t>
+  </si>
+  <si>
+    <t>https://image.wedmegood.com/resized/450X/uploads/project/1454/1439182065_IMG_2906.JPG</t>
+  </si>
+  <si>
+    <t>https://image.wedmegood.com/resized/450X/uploads/project/8711/1472478658_13265926_10154832363738222_9216591246948716119_n.jpg</t>
+  </si>
+  <si>
+    <t>https://image.wedmegood.com/resized/450X/uploads/project/20246/1526591357_30762714_2017645688562010_9202978509931151360_n.jpg</t>
+  </si>
+  <si>
+    <t>https://image.wedmegood.com/resized/450X/uploads/member/12191/1429696411_upo.jpg</t>
+  </si>
+  <si>
+    <t>contactNo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balaji Garden in Indore, also known as Shree Balaji Mangal Parisar, is a well-regarded wedding venue situated in Gumasta Nagar. This venue offers a spacious lawn that can accommodate up to 1,000 guests, making it ideal for large gatherings and weddings. The lush green lawn provides a serene backdrop, perfect for outdoor ceremonies and receptions​ </t>
+  </si>
+  <si>
+    <t>Raj Hans Garden</t>
   </si>
 </sst>
 </file>
@@ -394,463 +451,505 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J307"/>
+  <dimension ref="A1:H307"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="24.6328125" customWidth="1"/>
-    <col min="3" max="3" width="80.1796875" customWidth="1"/>
-    <col min="4" max="4" width="20.81640625" customWidth="1"/>
-    <col min="6" max="6" width="51" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" customWidth="1"/>
+    <col min="6" max="6" width="83.7265625" customWidth="1"/>
+    <col min="7" max="7" width="36.26953125" customWidth="1"/>
+    <col min="11" max="11" width="25.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="7">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2">
+        <v>500</v>
+      </c>
+      <c r="D2">
+        <v>8889344700</v>
+      </c>
+      <c r="E2" s="7">
         <v>40000</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="5">
+      <c r="F2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="5">
         <v>4.3</v>
       </c>
-      <c r="F2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>700</v>
+      </c>
+      <c r="D3">
+        <v>9993706123</v>
+      </c>
+      <c r="E3" s="7">
         <v>70000</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="5">
+      <c r="F3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="5">
         <v>3.3</v>
       </c>
-      <c r="F3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4">
+        <v>1000</v>
+      </c>
+      <c r="D4">
+        <v>9990744744</v>
+      </c>
+      <c r="E4" s="7">
         <v>50000</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="5">
+      <c r="F4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="5">
         <v>5</v>
       </c>
-      <c r="F4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <v>5000</v>
+      </c>
+      <c r="D5">
+        <v>8228690033</v>
+      </c>
+      <c r="E5" s="7">
         <v>30000</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="5">
+      <c r="F5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="5">
         <v>2.9</v>
       </c>
-      <c r="F5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6">
+        <v>800</v>
+      </c>
+      <c r="D6">
+        <v>8779390055</v>
+      </c>
+      <c r="E6" s="7">
         <v>450000</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="5">
+      <c r="F6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="5">
         <v>5</v>
       </c>
-      <c r="F6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7">
+        <v>10000</v>
+      </c>
+      <c r="D7">
+        <v>8580897517</v>
+      </c>
+      <c r="E7" s="7">
         <v>362000</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="5">
+      <c r="F7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="5">
         <v>4.0999999999999996</v>
       </c>
-      <c r="F7" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8">
+        <v>2000</v>
+      </c>
+      <c r="D8">
+        <v>8382404979</v>
+      </c>
+      <c r="E8" s="7">
         <v>440000</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="5">
+      <c r="F8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="5">
         <v>3.2</v>
       </c>
-      <c r="F8" t="s">
-        <v>24</v>
-      </c>
-      <c r="J8">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9">
+        <v>2400</v>
+      </c>
+      <c r="D9">
+        <v>8183912441</v>
+      </c>
+      <c r="E9" s="7">
         <v>518000</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="5">
+      <c r="F9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="5">
         <v>4.5</v>
       </c>
-      <c r="F9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J9">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10">
+        <v>5400</v>
+      </c>
+      <c r="D10">
+        <v>7985419903</v>
+      </c>
+      <c r="E10" s="7">
         <v>596000</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="5">
+      <c r="F10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="5">
         <v>5</v>
       </c>
-      <c r="F10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J10">
-        <v>5400</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11">
+        <v>3800</v>
+      </c>
+      <c r="D11">
+        <v>7786927365</v>
+      </c>
+      <c r="E11" s="7">
         <v>674000</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="5">
+      <c r="F11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="5">
         <v>2</v>
       </c>
-      <c r="F11" t="s">
-        <v>24</v>
-      </c>
-      <c r="J11">
-        <v>3800</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12">
+        <v>3200</v>
+      </c>
+      <c r="D12">
+        <v>7588434827</v>
+      </c>
+      <c r="E12" s="7">
         <v>752000</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="5">
+      <c r="F12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="5">
         <v>5</v>
       </c>
-      <c r="F12" t="s">
-        <v>24</v>
-      </c>
-      <c r="J12">
-        <v>3200</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13">
+        <v>1300</v>
+      </c>
+      <c r="D13">
+        <v>7389942289</v>
+      </c>
+      <c r="E13" s="7">
         <v>830000</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="5">
+      <c r="F13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="5">
         <v>3</v>
       </c>
-      <c r="F13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J13">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14">
+        <v>5000</v>
+      </c>
+      <c r="D14">
+        <v>7191449751</v>
+      </c>
+      <c r="E14" s="7">
         <v>908000</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="5">
+      <c r="F14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="5">
         <v>4</v>
       </c>
-      <c r="F14" t="s">
-        <v>24</v>
-      </c>
-      <c r="J14">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15">
+        <v>6000</v>
+      </c>
+      <c r="D15">
+        <v>6992957213</v>
+      </c>
+      <c r="E15" s="7">
         <v>986000</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="5">
+      <c r="F15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15" s="5">
         <v>3</v>
       </c>
-      <c r="F15" t="s">
-        <v>24</v>
-      </c>
-      <c r="J15">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="7">
+    </row>
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16">
+        <v>7000</v>
+      </c>
+      <c r="D16">
+        <v>6794464675</v>
+      </c>
+      <c r="E16" s="7">
         <v>1064000</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="5">
+      <c r="F16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" s="5">
         <v>5</v>
-      </c>
-      <c r="F16" t="s">
-        <v>24</v>
-      </c>
-      <c r="J16">
-        <v>7000</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="8"/>
+      <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="8"/>
+      <c r="C18" s="2"/>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
-      <c r="C19" s="8"/>
+      <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="8"/>
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
-      <c r="C21" s="8"/>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
-      <c r="C22" s="8"/>
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
       <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
       <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
-      <c r="C28" s="2"/>
       <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Click to Open WhatsApp/Phone/Email Directly
</commit_message>
<xml_diff>
--- a/back-end/Garden/GardenData.xlsx
+++ b/back-end/Garden/GardenData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DeadZoneMajorProject\wedding_planner\back-end\Garden\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3A48AC-38A8-47CA-AA9A-B88BFD096ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD43F91-9D82-4EBC-898E-9A8EC0FFB6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -454,7 +454,7 @@
   <dimension ref="A1:H307"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -505,7 +505,7 @@
         <v>500</v>
       </c>
       <c r="D2">
-        <v>8889344700</v>
+        <v>9302318373</v>
       </c>
       <c r="E2" s="7">
         <v>40000</v>
@@ -531,7 +531,7 @@
         <v>700</v>
       </c>
       <c r="D3">
-        <v>9993706123</v>
+        <v>9302558280</v>
       </c>
       <c r="E3" s="7">
         <v>70000</v>
@@ -557,7 +557,7 @@
         <v>1000</v>
       </c>
       <c r="D4">
-        <v>9990744744</v>
+        <v>8770155914</v>
       </c>
       <c r="E4" s="7">
         <v>50000</v>

</xml_diff>

<commit_message>
AddInBulkVendor SignIn Data Functionally addedd...
</commit_message>
<xml_diff>
--- a/back-end/Garden/GardenData.xlsx
+++ b/back-end/Garden/GardenData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DeadZoneMajorProject\wedding_planner\back-end\Garden\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DeadZone\wedding_planner\back-end\Garden\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD43F91-9D82-4EBC-898E-9A8EC0FFB6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1965C7-38DE-4D38-9247-749F3A9E5E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
   <si>
     <t>imageUrl</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>Raj Hans Garden</t>
+  </si>
+  <si>
+    <t>gardenId</t>
   </si>
 </sst>
 </file>
@@ -451,436 +454,484 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H307"/>
+  <dimension ref="A1:I307"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="24.6328125" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" customWidth="1"/>
+    <col min="3" max="3" width="27.54296875" customWidth="1"/>
     <col min="4" max="4" width="17.1796875" customWidth="1"/>
-    <col min="6" max="6" width="83.7265625" customWidth="1"/>
-    <col min="7" max="7" width="36.26953125" customWidth="1"/>
+    <col min="6" max="6" width="13.26953125" customWidth="1"/>
+    <col min="7" max="7" width="56.54296875" customWidth="1"/>
     <col min="11" max="11" width="25.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>500</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>9302318373</v>
       </c>
-      <c r="E2" s="7">
+      <c r="F2" s="7">
         <v>40000</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="5">
+      <c r="I2" s="5">
         <v>4.3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>700</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>9302558280</v>
       </c>
-      <c r="E3" s="7">
+      <c r="F3" s="7">
         <v>70000</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="5">
+      <c r="I3" s="5">
         <v>3.3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>1000</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>8770155914</v>
       </c>
-      <c r="E4" s="7">
+      <c r="F4" s="7">
         <v>50000</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>45</v>
       </c>
-      <c r="H4" s="5">
+      <c r="I4" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>5000</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>8228690033</v>
       </c>
-      <c r="E5" s="7">
+      <c r="F5" s="7">
         <v>30000</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>45</v>
       </c>
-      <c r="H5" s="5">
+      <c r="I5" s="5">
         <v>2.9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>800</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>8779390055</v>
       </c>
-      <c r="E6" s="7">
+      <c r="F6" s="7">
         <v>450000</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="5">
+      <c r="I6" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>24</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>10000</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>8580897517</v>
       </c>
-      <c r="E7" s="7">
+      <c r="F7" s="7">
         <v>362000</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="5">
+      <c r="I7" s="5">
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>25</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>2000</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>8382404979</v>
       </c>
-      <c r="E8" s="7">
+      <c r="F8" s="7">
         <v>440000</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>45</v>
       </c>
-      <c r="H8" s="5">
+      <c r="I8" s="5">
         <v>3.2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>26</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>2400</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>8183912441</v>
       </c>
-      <c r="E9" s="7">
+      <c r="F9" s="7">
         <v>518000</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>45</v>
       </c>
-      <c r="H9" s="5">
+      <c r="I9" s="5">
         <v>4.5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>27</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>5400</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>7985419903</v>
       </c>
-      <c r="E10" s="7">
+      <c r="F10" s="7">
         <v>596000</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>45</v>
       </c>
-      <c r="H10" s="5">
+      <c r="I10" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>28</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>3800</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>7786927365</v>
       </c>
-      <c r="E11" s="7">
+      <c r="F11" s="7">
         <v>674000</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="5">
+      <c r="I11" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>29</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>3200</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>7588434827</v>
       </c>
-      <c r="E12" s="7">
+      <c r="F12" s="7">
         <v>752000</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>45</v>
       </c>
-      <c r="H12" s="5">
+      <c r="I12" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>30</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>1300</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>7389942289</v>
       </c>
-      <c r="E13" s="7">
+      <c r="F13" s="7">
         <v>830000</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>45</v>
       </c>
-      <c r="H13" s="5">
+      <c r="I13" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>31</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>5000</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>7191449751</v>
       </c>
-      <c r="E14" s="7">
+      <c r="F14" s="7">
         <v>908000</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>45</v>
       </c>
-      <c r="H14" s="5">
+      <c r="I14" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>32</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>6000</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>6992957213</v>
       </c>
-      <c r="E15" s="7">
+      <c r="F15" s="7">
         <v>986000</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>45</v>
       </c>
-      <c r="H15" s="5">
+      <c r="I15" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>33</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>7000</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>6794464675</v>
       </c>
-      <c r="E16" s="7">
+      <c r="F16" s="7">
         <v>1064000</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="G16" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>45</v>
       </c>
-      <c r="H16" s="5">
+      <c r="I16" s="5">
         <v>5</v>
       </c>
     </row>
@@ -904,87 +955,71 @@
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
       <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
       <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
       <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
       <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
       <c r="C30" s="2"/>
       <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
       <c r="C31" s="3"/>
       <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
       <c r="C32" s="2"/>
       <c r="D32" s="3"/>
     </row>
     <row r="33" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
-      <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
       <c r="C34" s="2"/>
       <c r="D34" s="3"/>
     </row>
     <row r="35" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>

</xml_diff>

<commit_message>
Sweet Alert in GardenDetailPage Added..
</commit_message>
<xml_diff>
--- a/back-end/Garden/GardenData.xlsx
+++ b/back-end/Garden/GardenData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DeadZone\wedding_planner\back-end\Garden\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1965C7-38DE-4D38-9247-749F3A9E5E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8A9270-C01D-4231-B4ED-472609A1F323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -170,7 +170,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -193,6 +193,13 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -211,10 +218,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -236,8 +244,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -457,7 +467,7 @@
   <dimension ref="A1:I307"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -935,75 +945,76 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="2"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="G26" s="9"/>
+    </row>
+    <row r="27" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="C30" s="2"/>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
       <c r="C31" s="3"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
       <c r="C32" s="2"/>
       <c r="D32" s="3"/>

</xml_diff>